<commit_message>
Consolidate ISIC codes to match industry consolidation
</commit_message>
<xml_diff>
--- a/InputData/io-model/URPbIC/Union Representation Perc by ISIC Code.xlsx
+++ b/InputData/io-model/URPbIC/Union Representation Perc by ISIC Code.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarrynna\Dropbox (CEA)\Energy Innovation IO\Deliverable IO files\Mexico\URPbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-mexico\InputData\io-model\URPbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB36794-14F0-444C-8C37-06961CB49E35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{111598D9-CA0B-488C-B665-0CB52396764C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
     <sheet name="BLS Mexico Data" sheetId="5" r:id="rId2"/>
     <sheet name="ISIC to BLS Map" sheetId="4" r:id="rId3"/>
-    <sheet name="URPbIC" sheetId="3" r:id="rId4"/>
+    <sheet name="Pre ISIC Consolidation" sheetId="6" r:id="rId4"/>
+    <sheet name="URPbIC" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,14 +36,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="131">
   <si>
     <t>URPbIC Union Representation Percentage by ISIC Code</t>
   </si>
@@ -418,12 +418,51 @@
   </si>
   <si>
     <t>U.S. Bureau of Labor Statistics</t>
+  </si>
+  <si>
+    <t>Pre ISIC Consolidation Employment (see io-model/BEbIC)</t>
+  </si>
+  <si>
+    <t>Unit: jobs</t>
+  </si>
+  <si>
+    <t>ISIC 41T57*</t>
+  </si>
+  <si>
+    <t>Unit: %</t>
+  </si>
+  <si>
+    <t>EU ISIC Consolidation</t>
+  </si>
+  <si>
+    <t>Default EPS ISIC Groupings</t>
+  </si>
+  <si>
+    <t>Mexico ISIC Groupings</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
+  <si>
+    <t>Labor Productivity*Jobs</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Union Representation Before ISIC Code Allocation</t>
+  </si>
+  <si>
+    <t>Weighted Union Representation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,7 +508,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,6 +524,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,7 +663,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -674,11 +719,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{2F0C8A8E-D31E-4F34-A1FB-A6290494DAD1}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
@@ -1011,24 +1062,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A80408-5795-454F-9839-1063721C3DFB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1036,59 +1087,59 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="3"/>
       <c r="C4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C5" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C7" s="14" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{960B19AE-4E9A-40CF-BAD1-6D41A1CBA3DC}"/>
+    <hyperlink ref="C6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E54066-9771-4F1F-BC4F-B237B3B66844}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.86328125" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" customWidth="1"/>
+    <col min="6" max="6" width="71.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="26" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>1984</v>
@@ -1097,7 +1148,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1108,7 +1159,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1119,7 +1170,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1130,7 +1181,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1141,7 +1192,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1152,7 +1203,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1163,7 +1214,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -1174,7 +1225,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1185,7 +1236,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1196,7 +1247,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1207,7 +1258,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1218,7 +1269,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1229,7 +1280,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1240,7 +1291,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1251,7 +1302,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1262,7 +1313,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1273,7 +1324,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -1284,7 +1335,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1295,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1306,7 +1357,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1317,7 +1368,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1328,7 +1379,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B24" s="16"/>
     </row>
   </sheetData>
@@ -1340,22 +1391,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855C059D-400C-4D6E-8760-7A1D889573C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
@@ -1369,7 +1420,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1382,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>38</v>
       </c>
@@ -1398,7 +1449,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="12" t="s">
         <v>37</v>
       </c>
@@ -1414,7 +1465,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1430,7 +1481,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1446,7 +1497,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1462,7 +1513,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1478,7 +1529,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1494,7 +1545,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1510,7 +1561,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1526,7 +1577,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -1542,7 +1593,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
@@ -1555,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1568,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>40</v>
       </c>
@@ -1584,7 +1635,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="12" t="s">
         <v>39</v>
       </c>
@@ -1600,7 +1651,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
@@ -1616,7 +1667,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="12" t="s">
         <v>42</v>
       </c>
@@ -1632,7 +1683,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1648,7 +1699,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -1661,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -1677,7 +1728,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -1693,7 +1744,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -1709,7 +1760,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
@@ -1725,7 +1776,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
@@ -1741,7 +1792,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>43</v>
       </c>
@@ -1757,7 +1808,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
         <v>44</v>
       </c>
@@ -1773,7 +1824,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="12" t="s">
         <v>45</v>
       </c>
@@ -1789,7 +1840,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
@@ -1805,7 +1856,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>19</v>
       </c>
@@ -1821,7 +1872,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>20</v>
       </c>
@@ -1837,7 +1888,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
@@ -1853,7 +1904,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
@@ -1869,7 +1920,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>23</v>
       </c>
@@ -1885,7 +1936,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>24</v>
       </c>
@@ -1901,7 +1952,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
@@ -1917,7 +1968,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>26</v>
       </c>
@@ -1933,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>27</v>
       </c>
@@ -1949,7 +2000,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>28</v>
       </c>
@@ -1965,7 +2016,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>29</v>
       </c>
@@ -1981,7 +2032,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>30</v>
       </c>
@@ -1997,7 +2048,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>31</v>
       </c>
@@ -2010,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>32</v>
       </c>
@@ -2029,29 +2080,1547 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967A55DF-A297-4213-AF7B-8CD84E93B1AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:AQ16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.46484375" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="27"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" t="s">
+        <v>15</v>
+      </c>
+      <c r="X2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>2936200</v>
+      </c>
+      <c r="C3">
+        <v>34384.244052017966</v>
+      </c>
+      <c r="D3">
+        <v>23515.755947982037</v>
+      </c>
+      <c r="E3">
+        <v>160500</v>
+      </c>
+      <c r="F3">
+        <v>166500</v>
+      </c>
+      <c r="G3">
+        <v>1126400</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>183900</v>
+      </c>
+      <c r="K3">
+        <v>32400</v>
+      </c>
+      <c r="L3">
+        <v>150601.46396519794</v>
+      </c>
+      <c r="M3">
+        <v>114798.53603480205</v>
+      </c>
+      <c r="N3">
+        <v>243400</v>
+      </c>
+      <c r="O3">
+        <v>112928.34222642469</v>
+      </c>
+      <c r="P3">
+        <v>83771.657773575324</v>
+      </c>
+      <c r="Q3">
+        <v>42853.329699590206</v>
+      </c>
+      <c r="R3">
+        <v>47346.670300409794</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>653900</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>2986900</v>
+      </c>
+      <c r="Z3">
+        <v>158621.46382176597</v>
+      </c>
+      <c r="AA3">
+        <v>4013.7009469626901</v>
+      </c>
+      <c r="AB3">
+        <v>75264.835231271383</v>
+      </c>
+      <c r="AC3">
+        <v>4401100</v>
+      </c>
+      <c r="AD3">
+        <v>4800000</v>
+      </c>
+      <c r="AE3">
+        <v>2331800</v>
+      </c>
+      <c r="AF3">
+        <v>1377100</v>
+      </c>
+      <c r="AG3">
+        <v>77600</v>
+      </c>
+      <c r="AH3">
+        <v>92600</v>
+      </c>
+      <c r="AI3">
+        <v>49600</v>
+      </c>
+      <c r="AJ3">
+        <v>311300</v>
+      </c>
+      <c r="AK3">
+        <v>445400</v>
+      </c>
+      <c r="AL3">
+        <v>5082400</v>
+      </c>
+      <c r="AM3">
+        <v>2713200</v>
+      </c>
+      <c r="AN3">
+        <v>2353500</v>
+      </c>
+      <c r="AO3">
+        <v>1117000</v>
+      </c>
+      <c r="AP3">
+        <v>587800</v>
+      </c>
+      <c r="AQ3">
+        <v>2475600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A5" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="27"/>
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="27"/>
+      <c r="AO5" s="27"/>
+      <c r="AP5" s="27"/>
+      <c r="AQ5" s="27"/>
+    </row>
+    <row r="6" spans="1:43" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="5">
+        <f t="array" ref="B7:AQ7">TRANSPOSE('ISIC to BLS Map'!D2:D43)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.49</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L7" s="22">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P7" s="25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q7" s="22">
+        <v>0.26</v>
+      </c>
+      <c r="R7" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="S7" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="T7" s="5">
+        <v>0</v>
+      </c>
+      <c r="U7" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="V7" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="W7" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="X7" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="Z7" s="22">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AA7" s="25">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AB7" s="23">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="AJ7" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="AM7" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AN7" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AO7" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="29"/>
+      <c r="AB8" s="29"/>
+      <c r="AC8" s="29"/>
+      <c r="AD8" s="29"/>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="29"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
+      <c r="AK8" s="29"/>
+      <c r="AL8" s="29"/>
+      <c r="AM8" s="29"/>
+      <c r="AN8" s="29"/>
+      <c r="AO8" s="29"/>
+      <c r="AP8" s="29"/>
+      <c r="AQ8" s="29"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A9" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="27"/>
+      <c r="AI9" s="27"/>
+      <c r="AJ9" s="27"/>
+      <c r="AK9" s="27"/>
+      <c r="AL9" s="27"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="27"/>
+      <c r="AP9" s="27"/>
+      <c r="AQ9" s="27"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A13" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
+      <c r="AJ13" s="27"/>
+      <c r="AK13" s="27"/>
+      <c r="AL13" s="27"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="27"/>
+      <c r="AO13" s="27"/>
+      <c r="AP13" s="27"/>
+      <c r="AQ13" s="27"/>
+    </row>
+    <row r="14" spans="1:43" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15">
+        <f>(B3*B7)/100</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:AQ15" si="0">(C3*C7)/100</f>
+        <v>168.48279585488802</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>65.844116654349705</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>786.45</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>815.85</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2027.52</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>294.24</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>90.72</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>421.68409910255423</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>158.09967911699457</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>117.28032088300546</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>111.41865721893453</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>61.550671390532735</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="0"/>
+        <v>850.07</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>3882.97</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="0"/>
+        <v>904.14234378406593</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="0"/>
+        <v>22.878095397687328</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="0"/>
+        <v>429.00956081824683</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="0"/>
+        <v>880.22</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="0"/>
+        <v>3840</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="0"/>
+        <v>4663.6000000000004</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" si="0"/>
+        <v>1239.3900000000001</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="0"/>
+        <v>46.56</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="0"/>
+        <v>55.56</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="0"/>
+        <v>29.76</v>
+      </c>
+      <c r="AJ15">
+        <f t="shared" si="0"/>
+        <v>622.6</v>
+      </c>
+      <c r="AK15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <f t="shared" si="0"/>
+        <v>3049.44</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="0"/>
+        <v>7868.28</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="0"/>
+        <v>13414.95</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="0"/>
+        <v>3239.3</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="30">
+        <f>IFERROR(SUMIFS($B15:$AQ15,$B$11:$AQ$11,B14)/SUMIFS($B3:$AQ3,$B$11:$AQ$11,B14),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="30">
+        <f t="shared" ref="C16:AQ16" si="1">IFERROR(SUMIFS($B15:$AQ15,$B$11:$AQ$11,C14)/SUMIFS($B3:$AQ3,$B$11:$AQ$11,C14),0)</f>
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="D16" s="30">
+        <f t="shared" si="1"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="E16" s="30">
+        <f t="shared" si="1"/>
+        <v>4.9000000000000007E-3</v>
+      </c>
+      <c r="F16" s="30">
+        <f t="shared" si="1"/>
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="G16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.8E-3</v>
+      </c>
+      <c r="H16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="K16" s="30">
+        <f t="shared" si="1"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="L16" s="30">
+        <f t="shared" si="1"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="M16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="P16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="Q16" s="30">
+        <f t="shared" si="1"/>
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="R16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="S16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-3</v>
+      </c>
+      <c r="X16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="30">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="Z16" s="30">
+        <f t="shared" si="1"/>
+        <v>5.6999999999999993E-3</v>
+      </c>
+      <c r="AA16" s="30">
+        <f t="shared" si="1"/>
+        <v>5.6999999999999985E-3</v>
+      </c>
+      <c r="AB16" s="30">
+        <f t="shared" si="1"/>
+        <v>5.6999999999999993E-3</v>
+      </c>
+      <c r="AC16" s="30">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AD16" s="30">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AE16" s="30">
+        <f t="shared" si="1"/>
+        <v>2E-3</v>
+      </c>
+      <c r="AF16" s="30">
+        <f t="shared" si="1"/>
+        <v>9.0000000000000008E-4</v>
+      </c>
+      <c r="AG16" s="30">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AH16" s="30">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AI16" s="30">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AJ16" s="30">
+        <f t="shared" si="1"/>
+        <v>2E-3</v>
+      </c>
+      <c r="AK16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AL16" s="30">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AM16" s="30">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="AN16" s="30">
+        <f t="shared" si="1"/>
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="AO16" s="30">
+        <f t="shared" si="1"/>
+        <v>2.9000000000000002E-3</v>
+      </c>
+      <c r="AP16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="43" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="43" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
@@ -2182,142 +3751,183 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:43" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" cm="1">
-        <f t="array" ref="B2:AQ2">TRANSPOSE('ISIC to BLS Map'!D2:D43)</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="22">
-        <v>0.49</v>
-      </c>
-      <c r="D2" s="23">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.49</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.49</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.18</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="L2" s="22">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="M2" s="23">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="22">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="P2" s="25">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="Q2" s="22">
-        <v>0.26</v>
-      </c>
-      <c r="R2" s="23">
-        <v>0.13</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="W2" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="X2" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="Z2" s="22">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="AA2" s="25">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="AB2" s="23">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="AC2" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="AD2" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="AE2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="AF2" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="AG2" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="AH2" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="AI2" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="AJ2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="AK2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="AM2" s="5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AN2" s="5">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="AO2" s="5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <f>'Pre ISIC Consolidation'!B16</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="20">
+        <f>'Pre ISIC Consolidation'!C16</f>
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="D2" s="21">
+        <f>'Pre ISIC Consolidation'!D16</f>
+        <v>2.8E-3</v>
+      </c>
+      <c r="E2" s="3">
+        <f>'Pre ISIC Consolidation'!E16</f>
+        <v>4.9000000000000007E-3</v>
+      </c>
+      <c r="F2" s="3">
+        <f>'Pre ISIC Consolidation'!F16</f>
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="G2" s="3">
+        <f>'Pre ISIC Consolidation'!G16</f>
+        <v>1.8E-3</v>
+      </c>
+      <c r="H2" s="3">
+        <f>'Pre ISIC Consolidation'!H16</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <f>'Pre ISIC Consolidation'!I16</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <f>'Pre ISIC Consolidation'!J16</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="K2" s="3">
+        <f>'Pre ISIC Consolidation'!K16</f>
+        <v>2.8E-3</v>
+      </c>
+      <c r="L2" s="20">
+        <f>'Pre ISIC Consolidation'!L16</f>
+        <v>2.8E-3</v>
+      </c>
+      <c r="M2" s="21">
+        <f>'Pre ISIC Consolidation'!M16</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <f>'Pre ISIC Consolidation'!N16</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="20">
+        <f>'Pre ISIC Consolidation'!O16</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="P2" s="24">
+        <f>'Pre ISIC Consolidation'!P16</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="Q2" s="20">
+        <f>'Pre ISIC Consolidation'!Q16</f>
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="R2" s="21">
+        <f>'Pre ISIC Consolidation'!R16</f>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="S2" s="3">
+        <f>'Pre ISIC Consolidation'!S16</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
+        <f>'Pre ISIC Consolidation'!T16</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <f>'Pre ISIC Consolidation'!U16</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <f>'Pre ISIC Consolidation'!V16</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="3">
+        <f>'Pre ISIC Consolidation'!W16</f>
+        <v>1.3000000000000002E-3</v>
+      </c>
+      <c r="X2" s="3">
+        <f>'Pre ISIC Consolidation'!X16</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3">
+        <f>'Pre ISIC Consolidation'!Y16</f>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="Z2" s="20">
+        <f>'Pre ISIC Consolidation'!Z16</f>
+        <v>5.6999999999999993E-3</v>
+      </c>
+      <c r="AA2" s="24">
+        <f>'Pre ISIC Consolidation'!AA16</f>
+        <v>5.6999999999999985E-3</v>
+      </c>
+      <c r="AB2" s="21">
+        <f>'Pre ISIC Consolidation'!AB16</f>
+        <v>5.6999999999999993E-3</v>
+      </c>
+      <c r="AC2" s="3">
+        <f>'Pre ISIC Consolidation'!AC16</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AD2" s="3">
+        <f>'Pre ISIC Consolidation'!AD16</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AE2" s="3">
+        <f>'Pre ISIC Consolidation'!AE16</f>
+        <v>2E-3</v>
+      </c>
+      <c r="AF2" s="3">
+        <f>'Pre ISIC Consolidation'!AF16</f>
+        <v>9.0000000000000008E-4</v>
+      </c>
+      <c r="AG2" s="3">
+        <f>'Pre ISIC Consolidation'!AG16</f>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AH2" s="3">
+        <f>'Pre ISIC Consolidation'!AH16</f>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AI2" s="3">
+        <f>'Pre ISIC Consolidation'!AI16</f>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AJ2" s="3">
+        <f>'Pre ISIC Consolidation'!AJ16</f>
+        <v>2E-3</v>
+      </c>
+      <c r="AK2" s="3">
+        <f>'Pre ISIC Consolidation'!AK16</f>
+        <v>0</v>
+      </c>
+      <c r="AL2" s="3">
+        <f>'Pre ISIC Consolidation'!AL16</f>
+        <v>6.0000000000000006E-4</v>
+      </c>
+      <c r="AM2" s="3">
+        <f>'Pre ISIC Consolidation'!AM16</f>
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="AN2" s="3">
+        <f>'Pre ISIC Consolidation'!AN16</f>
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="AO2" s="3">
+        <f>'Pre ISIC Consolidation'!AO16</f>
+        <v>2.9000000000000002E-3</v>
+      </c>
+      <c r="AP2" s="3">
+        <f>'Pre ISIC Consolidation'!AP16</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="3">
+        <f>'Pre ISIC Consolidation'!AQ16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
       <c r="AE3" s="7"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -2326,7 +3936,7 @@
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B7" s="18"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -2335,7 +3945,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -2344,7 +3954,7 @@
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -2353,7 +3963,7 @@
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -2362,7 +3972,7 @@
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -2371,7 +3981,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -2380,7 +3990,7 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -2389,7 +3999,7 @@
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -2398,7 +4008,7 @@
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2407,7 +4017,7 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B16" s="19"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -2416,7 +4026,7 @@
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -2425,7 +4035,7 @@
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -2434,7 +4044,7 @@
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -2443,7 +4053,7 @@
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -2452,7 +4062,7 @@
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -2461,7 +4071,7 @@
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -2470,7 +4080,7 @@
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -2479,7 +4089,7 @@
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -2488,7 +4098,7 @@
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -2497,7 +4107,7 @@
       <c r="G25" s="17"/>
       <c r="H25" s="17"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -2506,7 +4116,7 @@
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -2515,7 +4125,7 @@
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -2524,7 +4134,7 @@
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -2533,7 +4143,7 @@
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -2542,7 +4152,7 @@
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -2551,7 +4161,7 @@
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -2560,7 +4170,7 @@
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -2569,7 +4179,7 @@
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -2578,7 +4188,7 @@
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -2587,7 +4197,7 @@
       <c r="G35" s="17"/>
       <c r="H35" s="17"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -2596,7 +4206,7 @@
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -2605,7 +4215,7 @@
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
@@ -2614,7 +4224,7 @@
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -2623,7 +4233,7 @@
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -2632,7 +4242,7 @@
       <c r="G40" s="17"/>
       <c r="H40" s="17"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -2641,7 +4251,7 @@
       <c r="G41" s="17"/>
       <c r="H41" s="17"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -2650,7 +4260,7 @@
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -2659,7 +4269,7 @@
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
@@ -2668,7 +4278,7 @@
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
@@ -2677,7 +4287,7 @@
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -2686,7 +4296,7 @@
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -2695,7 +4305,7 @@
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -2704,7 +4314,7 @@
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -2713,7 +4323,7 @@
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
@@ -2722,7 +4332,7 @@
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
@@ -2731,7 +4341,7 @@
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
@@ -2740,7 +4350,7 @@
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
@@ -2749,7 +4359,7 @@
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
@@ -2758,7 +4368,7 @@
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
@@ -2767,7 +4377,7 @@
       <c r="G55" s="17"/>
       <c r="H55" s="17"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
@@ -2776,7 +4386,7 @@
       <c r="G56" s="17"/>
       <c r="H56" s="17"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
@@ -2785,7 +4395,7 @@
       <c r="G57" s="17"/>
       <c r="H57" s="17"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
@@ -2794,7 +4404,7 @@
       <c r="G58" s="17"/>
       <c r="H58" s="17"/>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
       <c r="D59" s="17"/>
@@ -2803,7 +4413,7 @@
       <c r="G59" s="17"/>
       <c r="H59" s="17"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
       <c r="D60" s="17"/>
@@ -2812,7 +4422,7 @@
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
@@ -2821,7 +4431,7 @@
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
@@ -2830,7 +4440,7 @@
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
       <c r="D63" s="17"/>
@@ -2839,7 +4449,7 @@
       <c r="G63" s="17"/>
       <c r="H63" s="17"/>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>

</xml_diff>